<commit_message>
New color scheme for Excel calculator
</commit_message>
<xml_diff>
--- a/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
+++ b/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ada5d3d1b8db9262/Repos/TheCloudScout/sentinel-pricing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ada5d3d1b8db9262/Repos/TheCloudScout/sentinel-pricing/excel-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{224BAEBF-6089-4EA9-AC66-640A649B9939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CED6EC10-DD12-493A-A1B5-7C862CBC0678}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{224BAEBF-6089-4EA9-AC66-640A649B9939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B68961D0-F51A-4724-B234-15AF39FDDEAB}"/>
   <bookViews>
-    <workbookView xWindow="24480" yWindow="8928" windowWidth="17340" windowHeight="13020" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
+    <workbookView xWindow="14388" yWindow="1896" windowWidth="26424" windowHeight="18276" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
-  <si>
-    <t>West Europe €</t>
-  </si>
   <si>
     <t>/GB</t>
   </si>
@@ -75,6 +72,9 @@
   <si>
     <t>Log Analytics / Azure Monitor</t>
   </si>
+  <si>
+    <t>West Europe [ € ]</t>
+  </si>
 </sst>
 </file>
 
@@ -83,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,8 +114,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,34 +146,40 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <color rgb="FF4CD275"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="20"/>
-      <color theme="4" tint="-0.249977111117893"/>
+      <sz val="22"/>
+      <color rgb="FF4CD275"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -163,11 +192,11 @@
     </border>
     <border>
       <left style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </left>
       <right/>
       <top style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -176,7 +205,7 @@
       <left/>
       <right/>
       <top style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -184,17 +213,17 @@
     <border>
       <left/>
       <right style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </right>
       <top style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </left>
       <right/>
       <top/>
@@ -204,7 +233,7 @@
     <border>
       <left/>
       <right style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </right>
       <top/>
       <bottom/>
@@ -212,12 +241,12 @@
     </border>
     <border>
       <left style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </left>
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -226,18 +255,18 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </right>
       <top/>
       <bottom style="thick">
-        <color theme="9"/>
+        <color rgb="FF8300FF"/>
       </bottom>
       <diagonal/>
     </border>
@@ -246,61 +275,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyProtection="1">
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -308,6 +341,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8300FF"/>
+      <color rgb="FF4CD275"/>
+      <color rgb="FF2869D2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -353,6 +393,9 @@
         <a:prstGeom prst="bentUpArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4CD275"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -413,6 +456,9 @@
         <a:prstGeom prst="bentUpArrow">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4CD275"/>
+        </a:solidFill>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -743,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED95EF94-B75F-4922-9169-E5C76D7BBAA1}">
   <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,495 +816,497 @@
     <col min="19" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B2" s="27" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="L3" s="3"/>
+    <row r="2" spans="2:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="2:12" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="29">
         <v>2.6819999999999999</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
+      <c r="D5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="14"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="10">
+      <c r="C7" s="29">
         <v>226.79</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="28">
         <v>100</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="12">
+      <c r="E7" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="19">
         <f>C7/C5</f>
         <v>84.560029828486208</v>
       </c>
-      <c r="I7" s="16" t="s">
-        <v>5</v>
+      <c r="I7" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="10">
+      <c r="C8" s="29">
         <v>425.8</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="28">
         <v>200</v>
       </c>
-      <c r="E8" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="12">
+      <c r="E8" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="19">
         <f>((C8-C7)/C5)+D7</f>
         <v>174.20208799403431</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>5</v>
+      <c r="I8" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="10">
+      <c r="C9" s="29">
         <v>624.80999999999995</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="28">
         <v>300</v>
       </c>
-      <c r="E9" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="12">
+      <c r="E9" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="19">
         <f>((C9-C8)/C5)+D8</f>
         <v>274.20208799403429</v>
       </c>
-      <c r="I9" s="16" t="s">
-        <v>5</v>
+      <c r="I9" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="10">
+      <c r="C10" s="29">
         <v>814.57</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="28">
         <v>400</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="12">
+      <c r="E10" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="19">
         <f>((C10-C9)/C5)+D9</f>
         <v>370.75316927665926</v>
       </c>
-      <c r="I10" s="16" t="s">
-        <v>5</v>
+      <c r="I10" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="10">
+      <c r="C11" s="29">
         <v>1000.86</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="28">
         <v>500</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="12">
+      <c r="E11" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="19">
         <f>((C11-C10)/C5)+D10</f>
         <v>469.45935868754657</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>5</v>
+      <c r="I11" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="10">
+      <c r="C12" s="29">
         <v>1967</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="28">
         <v>1000</v>
       </c>
-      <c r="E12" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="12">
+      <c r="E12" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="19">
         <f>((C12-C11)/C5)+D11</f>
         <v>860.23117076808353</v>
       </c>
-      <c r="I12" s="16" t="s">
-        <v>5</v>
+      <c r="I12" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="10">
+      <c r="C13" s="29">
         <v>3841.43</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="28">
         <v>2000</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="12">
+      <c r="E13" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="19">
         <f>((C13-C12)/C5)+D12</f>
         <v>1698.8926174496644</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>5</v>
+      <c r="I13" s="20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="10">
+      <c r="C14" s="29">
         <v>9314.2900000000009</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="28">
         <v>5000</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="E14" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="22">
         <f>((C14-C13)/C5)+D13</f>
         <v>4040.5891126025354</v>
       </c>
-      <c r="I14" s="19" t="s">
-        <v>5</v>
+      <c r="I14" s="23" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="10"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="7"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C16" s="10"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K17" s="28" t="s">
-        <v>10</v>
+      <c r="E17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="10">
+      <c r="B20" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="29">
         <v>2.34</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24"/>
-      <c r="G20" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
+      <c r="D20" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="28"/>
+      <c r="G20" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="14"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C22" s="10">
+      <c r="C22" s="29">
         <v>117</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="28">
         <v>100</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="20">
+      <c r="E22" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="24">
         <f>C22/C20</f>
         <v>50</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>5</v>
+      <c r="I22" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J22" s="1"/>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C23" s="10">
+      <c r="C23" s="29">
         <v>210</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23" s="28">
         <v>200</v>
       </c>
-      <c r="E23" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H23" s="20">
+      <c r="E23" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="24">
         <f>((C23-C22)/C20)+D22</f>
         <v>139.74358974358975</v>
       </c>
-      <c r="I23" s="16" t="s">
-        <v>5</v>
+      <c r="I23" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J23" s="1"/>
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C24" s="10">
+      <c r="C24" s="29">
         <v>304</v>
       </c>
-      <c r="D24" s="24">
+      <c r="D24" s="28">
         <v>300</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H24" s="20">
+      <c r="E24" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="24">
         <f>((C24-C23)/C20)+D23</f>
         <v>240.17094017094018</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>5</v>
+      <c r="I24" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J24" s="1"/>
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C25" s="10">
+      <c r="C25" s="29">
         <v>389</v>
       </c>
-      <c r="D25" s="24">
+      <c r="D25" s="28">
         <v>400</v>
       </c>
-      <c r="E25" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H25" s="20">
+      <c r="E25" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="24">
         <f>((C25-C24)/C20)+D24</f>
         <v>336.32478632478632</v>
       </c>
-      <c r="I25" s="16" t="s">
-        <v>5</v>
+      <c r="I25" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J25" s="1"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C26" s="10">
+      <c r="C26" s="29">
         <v>467</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26" s="28">
         <v>500</v>
       </c>
-      <c r="E26" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="20">
+      <c r="E26" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="24">
         <f>((C26-C25)/C20)+D25</f>
         <v>433.33333333333331</v>
       </c>
-      <c r="I26" s="16" t="s">
-        <v>5</v>
+      <c r="I26" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J26" s="1"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C27" s="10">
+      <c r="C27" s="29">
         <v>910</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="28">
         <v>1000</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H27" s="20">
+      <c r="E27" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="24">
         <f>((C27-C26)/C20)+D26</f>
         <v>689.31623931623926</v>
       </c>
-      <c r="I27" s="16" t="s">
-        <v>5</v>
+      <c r="I27" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J27" s="1"/>
       <c r="N27" s="1"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C28" s="10">
+      <c r="C28" s="29">
         <v>1726</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28" s="28">
         <v>2000</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H28" s="20">
+      <c r="E28" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="24">
         <f>((C28-C27)/C20)+D27</f>
         <v>1348.7179487179487</v>
       </c>
-      <c r="I28" s="16" t="s">
-        <v>5</v>
+      <c r="I28" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="J28" s="1"/>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="10">
+      <c r="C29" s="29">
         <v>4082</v>
       </c>
-      <c r="D29" s="24">
+      <c r="D29" s="28">
         <v>5000</v>
       </c>
-      <c r="E29" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="H29" s="22">
+      <c r="E29" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="26">
         <f>((C29-C28)/C20)+D28</f>
         <v>3006.8376068376069</v>
       </c>
-      <c r="I29" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="L29" s="8"/>
+      <c r="I29" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="10"/>
     </row>
     <row r="30" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="10"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C31" s="10"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="5"/>
+      <c r="C31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="7"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="E32" s="4" t="s">
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="K32" s="28" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="9"/>
-      <c r="L34" s="8"/>
+      <c r="C34" s="11"/>
+      <c r="L34" s="10"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="9"/>
-      <c r="L35" s="8"/>
+      <c r="C35" s="11"/>
+      <c r="L35" s="10"/>
     </row>
     <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="9"/>
-      <c r="L36" s="8"/>
+      <c r="C36" s="11"/>
+      <c r="L36" s="10"/>
     </row>
     <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="9"/>
-      <c r="L37" s="9"/>
+      <c r="C37" s="11"/>
+      <c r="L37" s="11"/>
     </row>
     <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="9"/>
-      <c r="L38" s="9"/>
+      <c r="C38" s="11"/>
+      <c r="L38" s="11"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>

</xml_diff>

<commit_message>
Corrected commitment tier calculations
</commit_message>
<xml_diff>
--- a/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
+++ b/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koos.Goossens\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koos/Repos/TheCloudScout/sentinel-pricing/excel-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C58EA5F-6362-4783-94A8-6E255210644F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71213A10-9871-3549-B64B-4107571F1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25020" yWindow="9684" windowWidth="17268" windowHeight="12960" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
+    <workbookView xWindow="30460" yWindow="7640" windowWidth="31480" windowHeight="19120" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="14">
   <si>
     <t>/GB</t>
   </si>
@@ -75,6 +75,9 @@
   <si>
     <t>West Europe [ € ]</t>
   </si>
+  <si>
+    <t>Price/GB</t>
+  </si>
 </sst>
 </file>
 
@@ -83,7 +86,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_ &quot;€&quot;\ * #,##0.00_ ;_ &quot;€&quot;\ * \-#,##0.00_ ;_ &quot;€&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +166,14 @@
       <b/>
       <sz val="22"/>
       <color rgb="FF4CD275"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,64 +286,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -789,249 +803,284 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED95EF94-B75F-4922-9169-E5C76D7BBAA1}">
   <dimension ref="B2:N38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.33203125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="59.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="2" customWidth="1"/>
     <col min="16" max="16" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:12" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="28" t="s">
+    <row r="4" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="25">
         <v>2.6819999999999999</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="23"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="31" t="s">
+      <c r="G5" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C6" s="27"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="14"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="26">
+      <c r="H5" s="31"/>
+      <c r="I5" s="32"/>
+      <c r="L5" s="34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C6" s="26"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C7" s="25">
         <v>226.79</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>100</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" s="16">
+      <c r="G7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="15">
         <f>C7/C5</f>
         <v>84.560029828486208</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C8" s="26">
+      <c r="I7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="33">
+        <f>(C7/D7)</f>
+        <v>2.2679</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C8" s="25">
         <v>425.8</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>200</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="16">
-        <f>((C8-C7)/C5)+D7</f>
-        <v>174.20208799403431</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C9" s="26">
+      <c r="G8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="15">
+        <f>((C8-C7)/L8)+D7</f>
+        <v>193.47581023954911</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L8" s="33">
+        <f>(C8/D8)</f>
+        <v>2.129</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C9" s="25">
         <v>624.80999999999995</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>300</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="16">
-        <f>((C9-C8)/C5)+D8</f>
-        <v>274.20208799403429</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C10" s="26">
+      <c r="G9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="15">
+        <f>((C9-C8)/L8)+D8</f>
+        <v>293.47581023954905</v>
+      </c>
+      <c r="I9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="33">
+        <f>(C9/D9)</f>
+        <v>2.0827</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C10" s="25">
         <v>814.57</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>400</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="16">
-        <f>((C10-C9)/C5)+D9</f>
-        <v>370.75316927665926</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C11" s="26">
+      <c r="G10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="15">
+        <f>((C10-C9)/L9)+D9</f>
+        <v>391.11249819945272</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="33">
+        <f>(C10/D10)</f>
+        <v>2.0364249999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C11" s="25">
         <v>1000.86</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>500</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="16">
-        <f>((C11-C10)/C5)+D10</f>
-        <v>469.45935868754657</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C12" s="26">
+      <c r="G11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="15">
+        <f>((C11-C10)/L10)+D10</f>
+        <v>491.47893980873346</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L11" s="33">
+        <f>(C11/D11)</f>
+        <v>2.0017200000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C12" s="25">
         <v>1967</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>1000</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="16">
-        <f>((C12-C11)/C5)+D11</f>
-        <v>860.23117076808353</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="26">
+      <c r="G12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="15">
+        <f>((C12-C11)/L11)+D11</f>
+        <v>982.65491677157638</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L12" s="33">
+        <f>(C12/D12)</f>
+        <v>1.9670000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C13" s="25">
         <v>3841.43</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>2000</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="16">
-        <f>((C13-C12)/C5)+D12</f>
-        <v>1698.8926174496644</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="26">
+      <c r="G13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="15">
+        <f>((C13-C12)/L12)+D12</f>
+        <v>1952.9384850025417</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="33">
+        <f>(C13/D13)</f>
+        <v>1.920715</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="25">
         <v>9314.2900000000009</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>5000</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="23" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="7"/>
-      <c r="G14" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="19">
-        <f>((C14-C13)/C5)+D13</f>
-        <v>4040.5891126025354</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="18">
+        <f>((C14-C13)/L13)+D13</f>
+        <v>4849.3868168885028</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="33">
+        <f>(C14/D14)</f>
+        <v>1.8628580000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1039,7 +1088,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1047,224 +1096,255 @@
       <c r="H16" s="9"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:14" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="28" t="s">
+    <row r="19" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="25">
         <v>2.34</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="G20" s="31" t="s">
+      <c r="E20" s="24"/>
+      <c r="G20" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="32"/>
-      <c r="I20" s="33"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C21" s="27"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C22" s="26">
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C21" s="26"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C22" s="25">
         <v>117</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="24">
         <v>100</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="21">
+      <c r="E22" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="20">
         <f>C22/C20</f>
         <v>50</v>
       </c>
-      <c r="I22" s="17" t="s">
+      <c r="I22" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J22" s="1"/>
+      <c r="L22" s="33">
+        <f>C22/D22</f>
+        <v>1.17</v>
+      </c>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C23" s="26">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C23" s="25">
         <v>210</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="24">
         <v>200</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="21">
-        <f>((C23-C22)/C20)+D22</f>
-        <v>139.74358974358975</v>
-      </c>
-      <c r="I23" s="17" t="s">
+      <c r="E23" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="20">
+        <f>((C23-C22)/L22)+D22</f>
+        <v>179.4871794871795</v>
+      </c>
+      <c r="I23" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J23" s="1"/>
+      <c r="L23" s="33">
+        <f>C23/D23</f>
+        <v>1.05</v>
+      </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C24" s="26">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C24" s="25">
         <v>304</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="24">
         <v>300</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H24" s="21">
-        <f>((C24-C23)/C20)+D23</f>
-        <v>240.17094017094018</v>
-      </c>
-      <c r="I24" s="17" t="s">
+      <c r="E24" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="20">
+        <f>((C24-C23)/L23)+D23</f>
+        <v>289.52380952380952</v>
+      </c>
+      <c r="I24" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J24" s="1"/>
+      <c r="L24" s="33">
+        <f>C24/D24</f>
+        <v>1.0133333333333334</v>
+      </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C25" s="26">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C25" s="25">
         <v>389</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="24">
         <v>400</v>
       </c>
-      <c r="E25" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H25" s="21">
-        <f>((C25-C24)/C20)+D24</f>
-        <v>336.32478632478632</v>
-      </c>
-      <c r="I25" s="17" t="s">
+      <c r="E25" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="20">
+        <f>((C25-C24)/L24)+D24</f>
+        <v>383.88157894736844</v>
+      </c>
+      <c r="I25" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J25" s="1"/>
+      <c r="L25" s="33">
+        <f>C25/D25</f>
+        <v>0.97250000000000003</v>
+      </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C26" s="26">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C26" s="25">
         <v>467</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="24">
         <v>500</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" s="21">
-        <f>((C26-C25)/C20)+D25</f>
-        <v>433.33333333333331</v>
-      </c>
-      <c r="I26" s="17" t="s">
+      <c r="E26" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H26" s="20">
+        <f>((C26-C25)/L25)+D25</f>
+        <v>480.2056555269923</v>
+      </c>
+      <c r="I26" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J26" s="1"/>
+      <c r="L26" s="33">
+        <f>C26/D26</f>
+        <v>0.93400000000000005</v>
+      </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C27" s="26">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C27" s="25">
         <v>910</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="24">
         <v>1000</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="21">
-        <f>((C27-C26)/C20)+D26</f>
-        <v>689.31623931623926</v>
-      </c>
-      <c r="I27" s="17" t="s">
+      <c r="E27" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="20">
+        <f>((C27-C26)/L26)+D26</f>
+        <v>974.30406852248393</v>
+      </c>
+      <c r="I27" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J27" s="1"/>
+      <c r="L27" s="33">
+        <f>C27/D27</f>
+        <v>0.91</v>
+      </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="C28" s="26">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="25">
         <v>1726</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="24">
         <v>2000</v>
       </c>
-      <c r="E28" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="H28" s="21">
-        <f>((C28-C27)/C20)+D27</f>
-        <v>1348.7179487179487</v>
-      </c>
-      <c r="I28" s="17" t="s">
+      <c r="E28" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="20">
+        <f>((C28-C27)/L27)+D27</f>
+        <v>1896.7032967032967</v>
+      </c>
+      <c r="I28" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J28" s="1"/>
+      <c r="L28" s="33">
+        <f>C28/D28</f>
+        <v>0.86299999999999999</v>
+      </c>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C29" s="26">
+    <row r="29" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="25">
         <v>4082</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="24">
         <v>5000</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="H29" s="23">
-        <f>((C29-C28)/C20)+D28</f>
-        <v>3006.8376068376069</v>
-      </c>
-      <c r="I29" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="10"/>
-    </row>
-    <row r="30" spans="2:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="22">
+        <f>((C29-C28)/L28)+D28</f>
+        <v>4730.0115874855155</v>
+      </c>
+      <c r="I29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="33">
+        <f>C29/D29</f>
+        <v>0.81640000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1272,7 +1352,7 @@
       <c r="H30" s="9"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1280,33 +1360,33 @@
       <c r="H31" s="9"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="E32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="29" t="s">
+      <c r="K32" s="28" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="11"/>
+    <row r="34" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C34" s="2"/>
       <c r="L34" s="10"/>
     </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C35" s="11"/>
+    <row r="35" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C35" s="2"/>
       <c r="L35" s="10"/>
     </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="11"/>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C36" s="2"/>
       <c r="L36" s="10"/>
     </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="11"/>
-      <c r="L37" s="11"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="11"/>
-      <c r="L38" s="11"/>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C38" s="2"/>
+      <c r="L38" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>

</xml_diff>

<commit_message>
Adjusted prices and thresholds at of May 26th 2023
</commit_message>
<xml_diff>
--- a/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
+++ b/excel-calculator/sentinel-pricing-tiers-and-recommendation-thresholds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koos/Repos/TheCloudScout/sentinel-pricing/excel-calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71213A10-9871-3549-B64B-4107571F1B33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062E3409-CFBE-9946-868B-852D6B733068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30460" yWindow="7640" windowWidth="31480" windowHeight="19120" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
+    <workbookView xWindow="28080" yWindow="1120" windowWidth="30260" windowHeight="21840" xr2:uid="{366AC0B3-F41D-41BF-BCD0-996990D88114}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
   <si>
     <t>/GB</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>West Europe [ € ]</t>
-  </si>
-  <si>
-    <t>Price/GB</t>
   </si>
 </sst>
 </file>
@@ -286,7 +283,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -317,9 +314,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -335,6 +329,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,10 +341,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -801,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED95EF94-B75F-4922-9169-E5C76D7BBAA1}">
-  <dimension ref="B2:N38"/>
+  <dimension ref="B2:R38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -820,66 +814,64 @@
     <col min="9" max="9" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.33203125" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" style="2" customWidth="1"/>
     <col min="16" max="16" width="2" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.5" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="B2" s="29" t="s">
+    <row r="2" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="4"/>
       <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:12" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="27" t="s">
+    <row r="4" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:18" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="25">
-        <v>2.6819999999999999</v>
-      </c>
-      <c r="D5" s="23" t="s">
+      <c r="C5" s="24">
+        <v>2.7080000000000002</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="22"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="L5" s="34" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C6" s="26"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="33"/>
+      <c r="L5" s="30"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C6" s="25"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
       <c r="G6" s="11"/>
       <c r="H6" s="12"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C7" s="25">
-        <v>226.79</v>
-      </c>
-      <c r="D7" s="24">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C7" s="24">
+        <v>228.95</v>
+      </c>
+      <c r="D7" s="23">
         <v>100</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F7" s="7"/>
@@ -888,24 +880,21 @@
       </c>
       <c r="H7" s="15">
         <f>C7/C5</f>
-        <v>84.560029828486208</v>
+        <v>84.545790251107817</v>
       </c>
       <c r="I7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="33">
-        <f>(C7/D7)</f>
-        <v>2.2679</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C8" s="25">
-        <v>425.8</v>
-      </c>
-      <c r="D8" s="24">
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C8" s="24">
+        <v>429.87</v>
+      </c>
+      <c r="D8" s="23">
         <v>200</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F8" s="7"/>
@@ -913,25 +902,23 @@
         <v>3</v>
       </c>
       <c r="H8" s="15">
-        <f>((C8-C7)/L8)+D7</f>
-        <v>193.47581023954911</v>
+        <f>C8/(C7/D7)</f>
+        <v>187.7571522166412</v>
       </c>
       <c r="I8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="33">
-        <f>(C8/D8)</f>
-        <v>2.129</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C9" s="25">
-        <v>624.80999999999995</v>
-      </c>
-      <c r="D9" s="24">
+      <c r="L8" s="29"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C9" s="24">
+        <v>630.78</v>
+      </c>
+      <c r="D9" s="23">
         <v>300</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F9" s="7"/>
@@ -939,25 +926,22 @@
         <v>3</v>
       </c>
       <c r="H9" s="15">
-        <f>((C9-C8)/L8)+D8</f>
-        <v>293.47581023954905</v>
+        <f>C9/(C8/D8)</f>
+        <v>293.47477144252912</v>
       </c>
       <c r="I9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="33">
-        <f>(C9/D9)</f>
-        <v>2.0827</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C10" s="25">
-        <v>814.57</v>
-      </c>
-      <c r="D10" s="24">
+      <c r="L9" s="29"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C10" s="24">
+        <v>822.35</v>
+      </c>
+      <c r="D10" s="23">
         <v>400</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F10" s="7"/>
@@ -965,25 +949,22 @@
         <v>3</v>
       </c>
       <c r="H10" s="15">
-        <f>((C10-C9)/L9)+D9</f>
-        <v>391.11249819945272</v>
+        <f t="shared" ref="H10:H14" si="0">C10/(C9/D9)</f>
+        <v>391.11100542185869</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="33">
-        <f>(C10/D10)</f>
-        <v>2.0364249999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="25">
-        <v>1000.86</v>
-      </c>
-      <c r="D11" s="24">
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C11" s="24">
+        <v>1010.42</v>
+      </c>
+      <c r="D11" s="23">
         <v>500</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F11" s="7"/>
@@ -991,25 +972,22 @@
         <v>3</v>
       </c>
       <c r="H11" s="15">
-        <f>((C11-C10)/L10)+D10</f>
-        <v>491.47893980873346</v>
+        <f t="shared" si="0"/>
+        <v>491.47929713625587</v>
       </c>
       <c r="I11" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L11" s="33">
-        <f>(C11/D11)</f>
-        <v>2.0017200000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="25">
-        <v>1967</v>
-      </c>
-      <c r="D12" s="24">
+      <c r="L11" s="29"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C12" s="24">
+        <v>1985.79</v>
+      </c>
+      <c r="D12" s="23">
         <v>1000</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F12" s="7"/>
@@ -1017,25 +995,22 @@
         <v>3</v>
       </c>
       <c r="H12" s="15">
-        <f>((C12-C11)/L11)+D11</f>
-        <v>982.65491677157638</v>
+        <f t="shared" si="0"/>
+        <v>982.65572732131204</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L12" s="33">
-        <f>(C12/D12)</f>
-        <v>1.9670000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="25">
-        <v>3841.43</v>
-      </c>
-      <c r="D13" s="24">
+      <c r="L12" s="29"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="C13" s="24">
+        <v>3878.12</v>
+      </c>
+      <c r="D13" s="23">
         <v>2000</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F13" s="7"/>
@@ -1043,44 +1018,38 @@
         <v>3</v>
       </c>
       <c r="H13" s="15">
-        <f>((C13-C12)/L12)+D12</f>
-        <v>1952.9384850025417</v>
+        <f t="shared" si="0"/>
+        <v>1952.9356074912253</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="L13" s="33">
-        <f>(C13/D13)</f>
-        <v>1.920715</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="25">
-        <v>9314.2900000000009</v>
-      </c>
-      <c r="D14" s="24">
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="2:18" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="24">
+        <v>9403.27</v>
+      </c>
+      <c r="D14" s="23">
         <v>5000</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>1</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="18">
-        <f>((C14-C13)/L13)+D13</f>
-        <v>4849.3868168885028</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="L14" s="33">
-        <f>(C14/D14)</f>
-        <v>1.8628580000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="21">
+        <f t="shared" si="0"/>
+        <v>4849.3960991408212</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="2:18" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1088,7 +1057,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="C16" s="6"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1096,255 +1065,232 @@
       <c r="H16" s="9"/>
       <c r="I16" s="7"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E17" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K17" s="28" t="s">
+      <c r="K17" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="27" t="s">
+    <row r="19" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="25">
-        <v>2.34</v>
-      </c>
-      <c r="D20" s="23" t="s">
+      <c r="C20" s="24">
+        <v>2.36</v>
+      </c>
+      <c r="D20" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="G20" s="30" t="s">
+      <c r="E20" s="23"/>
+      <c r="G20" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="31"/>
-      <c r="I20" s="32"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="26"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="33"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C21" s="25"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="G21" s="11"/>
       <c r="H21" s="12"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="25">
-        <v>117</v>
-      </c>
-      <c r="D22" s="24">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C22" s="24">
+        <v>117.72</v>
+      </c>
+      <c r="D22" s="23">
         <v>100</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="19">
         <f>C22/C20</f>
-        <v>50</v>
+        <v>49.881355932203391</v>
       </c>
       <c r="I22" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J22" s="1"/>
-      <c r="L22" s="33">
-        <f>C22/D22</f>
-        <v>1.17</v>
-      </c>
+      <c r="L22" s="29"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C23" s="25">
-        <v>210</v>
-      </c>
-      <c r="D23" s="24">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C23" s="24">
+        <v>211.89</v>
+      </c>
+      <c r="D23" s="23">
         <v>200</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H23" s="20">
-        <f>((C23-C22)/L22)+D22</f>
-        <v>179.4871794871795</v>
+      <c r="H23" s="19">
+        <f>C23/(C22/D22)</f>
+        <v>179.99490316004076</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J23" s="1"/>
-      <c r="L23" s="33">
-        <f>C23/D23</f>
-        <v>1.05</v>
-      </c>
+      <c r="L23" s="29"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="25">
-        <v>304</v>
-      </c>
-      <c r="D24" s="24">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C24" s="24">
+        <v>306.07</v>
+      </c>
+      <c r="D24" s="23">
         <v>300</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="20">
-        <f>((C24-C23)/L23)+D23</f>
-        <v>289.52380952380952</v>
+      <c r="H24" s="19">
+        <f t="shared" ref="H24:H29" si="1">C24/(C23/D23)</f>
+        <v>288.89518146207939</v>
       </c>
       <c r="I24" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J24" s="1"/>
-      <c r="L24" s="33">
-        <f>C24/D24</f>
-        <v>1.0133333333333334</v>
-      </c>
+      <c r="L24" s="29"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="25">
-        <v>389</v>
-      </c>
-      <c r="D25" s="24">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C25" s="24">
+        <v>392.39</v>
+      </c>
+      <c r="D25" s="23">
         <v>400</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="20">
-        <f>((C25-C24)/L24)+D24</f>
-        <v>383.88157894736844</v>
+      <c r="H25" s="19">
+        <f t="shared" si="1"/>
+        <v>384.60809618714671</v>
       </c>
       <c r="I25" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J25" s="1"/>
-      <c r="L25" s="33">
-        <f>C25/D25</f>
-        <v>0.97250000000000003</v>
-      </c>
+      <c r="L25" s="29"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="25">
-        <v>467</v>
-      </c>
-      <c r="D26" s="24">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C26" s="24">
+        <v>470.87</v>
+      </c>
+      <c r="D26" s="23">
         <v>500</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="20">
-        <f>((C26-C25)/L25)+D25</f>
-        <v>480.2056555269923</v>
+      <c r="H26" s="19">
+        <f t="shared" si="1"/>
+        <v>480.00203878794059</v>
       </c>
       <c r="I26" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J26" s="1"/>
-      <c r="L26" s="33">
-        <f>C26/D26</f>
-        <v>0.93400000000000005</v>
-      </c>
+      <c r="L26" s="29"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="25">
-        <v>910</v>
-      </c>
-      <c r="D27" s="24">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C27" s="24">
+        <v>918.19</v>
+      </c>
+      <c r="D27" s="23">
         <v>1000</v>
       </c>
-      <c r="E27" s="23" t="s">
+      <c r="E27" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="20">
-        <f>((C27-C26)/L26)+D26</f>
-        <v>974.30406852248393</v>
+      <c r="H27" s="19">
+        <f t="shared" si="1"/>
+        <v>974.99309788264281</v>
       </c>
       <c r="I27" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J27" s="1"/>
-      <c r="L27" s="33">
-        <f>C27/D27</f>
-        <v>0.91</v>
-      </c>
+      <c r="L27" s="29"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="25">
-        <v>1726</v>
-      </c>
-      <c r="D28" s="24">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C28" s="24">
+        <v>1742.21</v>
+      </c>
+      <c r="D28" s="23">
         <v>2000</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>1</v>
       </c>
       <c r="G28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H28" s="20">
-        <f>((C28-C27)/L27)+D27</f>
-        <v>1896.7032967032967</v>
+      <c r="H28" s="19">
+        <f t="shared" si="1"/>
+        <v>1897.4395277665842</v>
       </c>
       <c r="I28" s="16" t="s">
         <v>4</v>
       </c>
       <c r="J28" s="1"/>
-      <c r="L28" s="33">
-        <f>C28/D28</f>
-        <v>0.86299999999999999</v>
-      </c>
+      <c r="L28" s="29"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="2:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="25">
-        <v>4082</v>
-      </c>
-      <c r="D29" s="24">
+    <row r="29" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="24">
+        <v>4120.08</v>
+      </c>
+      <c r="D29" s="23">
         <v>5000</v>
       </c>
-      <c r="E29" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="H29" s="22">
-        <f>((C29-C28)/L28)+D28</f>
-        <v>4730.0115874855155</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="L29" s="33">
-        <f>C29/D29</f>
-        <v>0.81640000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="21">
+        <f t="shared" si="1"/>
+        <v>4729.7168538809901</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="L29" s="29"/>
+      <c r="Q29" s="10"/>
+    </row>
+    <row r="30" spans="2:17" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C30" s="6"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -1352,7 +1298,7 @@
       <c r="H30" s="9"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C31" s="6"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -1360,11 +1306,11 @@
       <c r="H31" s="9"/>
       <c r="I31" s="7"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K32" s="28" t="s">
+      <c r="K32" s="27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1389,7 +1335,7 @@
       <c r="L38" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G20:I20"/>
@@ -1403,4 +1349,10 @@
   <pageSetup orientation="portrait" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{a51cdf94-b825-48c2-8b27-51ed6f9320b0}" enabled="1" method="Privileged" siteId="{b1a6616c-9473-4cab-82b6-b6affeed3e12}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>